<commit_message>
ansemble method + structurized results
</commit_message>
<xml_diff>
--- a/anextour parser/parsed.xlsx
+++ b/anextour parser/parsed.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dipl\anextour parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298D639F-A37D-4B60-8592-6960C3F139E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389330C5-7FD0-41F2-B91A-47B3543B1AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="1050" windowWidth="30660" windowHeight="19590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="30660" windowHeight="19590" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="вопросы" sheetId="2" r:id="rId2"/>
     <sheet name="вопросы прямые(ds1)" sheetId="4" r:id="rId3"/>
     <sheet name="вопросы синонимы(ds2)" sheetId="3" r:id="rId4"/>
-    <sheet name="вопросы близкие по контексту" sheetId="5" r:id="rId5"/>
-    <sheet name="вопросы далекие от контекста" sheetId="6" r:id="rId6"/>
+    <sheet name="запрос простыми словами(ds3)" sheetId="7" r:id="rId5"/>
+    <sheet name="вопросы близкие по контексту" sheetId="5" r:id="rId6"/>
+    <sheet name="вопросы далекие от контекста" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$G$1:$G$227</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1540" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1607" uniqueCount="993">
   <si>
     <t>Золотая Москва (лето)</t>
   </si>
@@ -2694,9 +2695,6 @@
     <t>иркутская обл.</t>
   </si>
   <si>
-    <t>126, 2, 6, 7, 26, 27, 28, 125</t>
-  </si>
-  <si>
     <t>relv</t>
   </si>
   <si>
@@ -2745,9 +2743,6 @@
     <t>тур на полуостров вулканов, включающий посещение горных массивов, а также различных водных объектов</t>
   </si>
   <si>
-    <t>46, 118, 119, 183, 184, 196, 212, 213, 214</t>
-  </si>
-  <si>
     <t xml:space="preserve">тур по Владивостоку с обзорной экскурсией по городу, посещением острова Русский и Приморского сафари-парка. </t>
   </si>
   <si>
@@ -2925,9 +2920,6 @@
     <t>160, 161, 162</t>
   </si>
   <si>
-    <t>62, 64, 65, 144, 163, 165, 179, 186, 187,</t>
-  </si>
-  <si>
     <t>ищу тур по Карачаево-Черкесия, включающий в себя горнолыжный курорт Домбай, а также экскурсии по Шоанинскому и Сентинскому храмам</t>
   </si>
   <si>
@@ -2950,6 +2942,81 @@
   </si>
   <si>
     <t>тур по столице марийской республики, влючающая посещение площадей и набережных с возможностью попробовать местную кухню</t>
+  </si>
+  <si>
+    <t>2, 3, 4, 5,  6, 7, 8, 23, 24, 25, 26, 27, 28, 125, 126, 201</t>
+  </si>
+  <si>
+    <t>46, 118, 119, 182, 183, 184, 196, 212, 213, 214</t>
+  </si>
+  <si>
+    <t>simple dimple</t>
+  </si>
+  <si>
+    <t>Экскурсионный тур СПб: Петергоф и Кронштадт в программе</t>
+  </si>
+  <si>
+    <t>Туры в Псковскую область: Псков и Пушкинские Горы</t>
+  </si>
+  <si>
+    <t>Экскурсионный тур по Владивостоку с походом в Сафари-парк</t>
+  </si>
+  <si>
+    <t>Туры в Карелию с посещением Центра Шунгита</t>
+  </si>
+  <si>
+    <t>фототур в Мурманск с наблюдением за китами</t>
+  </si>
+  <si>
+    <t>Тур на Камчатку: вулканы, термальные источники и морские экскурсии</t>
+  </si>
+  <si>
+    <t>Тур на Сахалин / Куриллы посмотреть море</t>
+  </si>
+  <si>
+    <t>Туры Сахалин - Курилы: горячие источники, прогулки по побережью</t>
+  </si>
+  <si>
+    <t>санатории калининградская область</t>
+  </si>
+  <si>
+    <t>обзорный тур по Великому Новгороду</t>
+  </si>
+  <si>
+    <t>тур в дом-музей Достоевского</t>
+  </si>
+  <si>
+    <t>обзорная экскурсия по Йошкар-оле</t>
+  </si>
+  <si>
+    <t>Ингушетия: тур в горные районы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Горнолыжный курорт Домбай Карачаево-Черкесия </t>
+  </si>
+  <si>
+    <t>экскурсия Чечня «Город Грозный – прошлое и настоящее»</t>
+  </si>
+  <si>
+    <t>тур по Москве с экскурсиями по Красной площади и т. П.</t>
+  </si>
+  <si>
+    <t>Дагестан: туры по республике с посещением аула-призрака Гамсутль</t>
+  </si>
+  <si>
+    <t>Экскурсионный тур в Калининград по городу, Куршской косе</t>
+  </si>
+  <si>
+    <t>Экскурсионный тур в Карелию в Кивач, Марциальные воды</t>
+  </si>
+  <si>
+    <t>Сибирский хайкинг тур  по горной гряде "Сундуки"</t>
+  </si>
+  <si>
+    <t>Тур на Байкал зимой</t>
+  </si>
+  <si>
+    <t>62, 64, 65, 144, 163, 165, 179, 186, 187</t>
   </si>
 </sst>
 </file>
@@ -3328,10 +3395,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D94" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView topLeftCell="C58" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3368,7 +3436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -3391,7 +3459,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3414,7 +3482,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -3437,7 +3505,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -3460,7 +3528,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -3483,7 +3551,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -3506,7 +3574,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -3529,7 +3597,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -3552,7 +3620,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -3575,7 +3643,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -3598,7 +3666,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -3621,7 +3689,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -3644,7 +3712,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -3667,7 +3735,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -3690,7 +3758,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -3713,7 +3781,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -3736,7 +3804,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>16</v>
       </c>
@@ -3759,7 +3827,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>17</v>
       </c>
@@ -3782,7 +3850,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>18</v>
       </c>
@@ -3805,7 +3873,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>19</v>
       </c>
@@ -3828,7 +3896,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>20</v>
       </c>
@@ -3851,7 +3919,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>21</v>
       </c>
@@ -3874,7 +3942,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>22</v>
       </c>
@@ -3897,7 +3965,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>23</v>
       </c>
@@ -3920,7 +3988,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>24</v>
       </c>
@@ -3943,7 +4011,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>25</v>
       </c>
@@ -3966,7 +4034,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>26</v>
       </c>
@@ -3989,7 +4057,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>27</v>
       </c>
@@ -4012,7 +4080,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -4035,7 +4103,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29</v>
       </c>
@@ -4058,7 +4126,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>30</v>
       </c>
@@ -4081,7 +4149,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>31</v>
       </c>
@@ -4104,7 +4172,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>32</v>
       </c>
@@ -4127,7 +4195,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>33</v>
       </c>
@@ -4150,7 +4218,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>34</v>
       </c>
@@ -4173,7 +4241,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>35</v>
       </c>
@@ -4219,7 +4287,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>37</v>
       </c>
@@ -4242,7 +4310,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>38</v>
       </c>
@@ -4265,7 +4333,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>39</v>
       </c>
@@ -4288,7 +4356,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>40</v>
       </c>
@@ -4380,7 +4448,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>44</v>
       </c>
@@ -4403,7 +4471,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45</v>
       </c>
@@ -4426,7 +4494,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>46</v>
       </c>
@@ -4449,7 +4517,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>47</v>
       </c>
@@ -4472,7 +4540,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>48</v>
       </c>
@@ -4564,7 +4632,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>52</v>
       </c>
@@ -4587,7 +4655,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>53</v>
       </c>
@@ -4610,7 +4678,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="375" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>54</v>
       </c>
@@ -4633,7 +4701,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>55</v>
       </c>
@@ -4702,7 +4770,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>58</v>
       </c>
@@ -4725,7 +4793,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>59</v>
       </c>
@@ -4748,7 +4816,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>60</v>
       </c>
@@ -4771,7 +4839,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>61</v>
       </c>
@@ -4794,7 +4862,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>62</v>
       </c>
@@ -4817,7 +4885,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>63</v>
       </c>
@@ -4840,7 +4908,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>64</v>
       </c>
@@ -4863,7 +4931,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>65</v>
       </c>
@@ -4886,7 +4954,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>66</v>
       </c>
@@ -4978,7 +5046,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>70</v>
       </c>
@@ -5001,7 +5069,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>71</v>
       </c>
@@ -5024,7 +5092,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>72</v>
       </c>
@@ -5047,7 +5115,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>73</v>
       </c>
@@ -5070,7 +5138,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>74</v>
       </c>
@@ -5093,7 +5161,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>75</v>
       </c>
@@ -5116,7 +5184,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>76</v>
       </c>
@@ -5139,7 +5207,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>77</v>
       </c>
@@ -5162,7 +5230,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>78</v>
       </c>
@@ -5185,7 +5253,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>79</v>
       </c>
@@ -5208,7 +5276,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>80</v>
       </c>
@@ -5231,7 +5299,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>81</v>
       </c>
@@ -5254,7 +5322,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>82</v>
       </c>
@@ -5277,7 +5345,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>83</v>
       </c>
@@ -5300,7 +5368,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>84</v>
       </c>
@@ -5323,7 +5391,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>85</v>
       </c>
@@ -5346,7 +5414,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>86</v>
       </c>
@@ -5369,7 +5437,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>87</v>
       </c>
@@ -5392,7 +5460,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>88</v>
       </c>
@@ -5415,7 +5483,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>89</v>
       </c>
@@ -5438,7 +5506,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>90</v>
       </c>
@@ -5461,7 +5529,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>91</v>
       </c>
@@ -5484,7 +5552,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>92</v>
       </c>
@@ -5507,7 +5575,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>93</v>
       </c>
@@ -5530,7 +5598,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>94</v>
       </c>
@@ -5553,7 +5621,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>95</v>
       </c>
@@ -5576,7 +5644,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>96</v>
       </c>
@@ -5599,7 +5667,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>97</v>
       </c>
@@ -5622,7 +5690,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>98</v>
       </c>
@@ -5645,7 +5713,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>99</v>
       </c>
@@ -5668,7 +5736,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>100</v>
       </c>
@@ -5691,7 +5759,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>101</v>
       </c>
@@ -5714,7 +5782,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>102</v>
       </c>
@@ -5737,7 +5805,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>103</v>
       </c>
@@ -5760,7 +5828,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>104</v>
       </c>
@@ -5783,7 +5851,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>105</v>
       </c>
@@ -5806,7 +5874,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>106</v>
       </c>
@@ -5829,7 +5897,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>107</v>
       </c>
@@ -5852,7 +5920,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>108</v>
       </c>
@@ -5875,7 +5943,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>109</v>
       </c>
@@ -5898,7 +5966,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>110</v>
       </c>
@@ -5921,7 +5989,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>111</v>
       </c>
@@ -5944,7 +6012,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>112</v>
       </c>
@@ -5990,7 +6058,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>114</v>
       </c>
@@ -6013,7 +6081,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>115</v>
       </c>
@@ -6036,7 +6104,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>116</v>
       </c>
@@ -6059,7 +6127,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>117</v>
       </c>
@@ -6082,7 +6150,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>118</v>
       </c>
@@ -6105,7 +6173,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>119</v>
       </c>
@@ -6197,7 +6265,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>123</v>
       </c>
@@ -6243,7 +6311,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>125</v>
       </c>
@@ -6266,7 +6334,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>126</v>
       </c>
@@ -6289,7 +6357,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>127</v>
       </c>
@@ -6312,7 +6380,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>128</v>
       </c>
@@ -6335,7 +6403,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>129</v>
       </c>
@@ -6358,7 +6426,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>130</v>
       </c>
@@ -6381,7 +6449,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>131</v>
       </c>
@@ -6404,7 +6472,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="375" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>132</v>
       </c>
@@ -6427,7 +6495,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>133</v>
       </c>
@@ -6450,7 +6518,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>134</v>
       </c>
@@ -6473,7 +6541,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>135</v>
       </c>
@@ -6496,7 +6564,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>136</v>
       </c>
@@ -6588,7 +6656,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>140</v>
       </c>
@@ -6611,7 +6679,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>141</v>
       </c>
@@ -6657,7 +6725,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>143</v>
       </c>
@@ -6680,7 +6748,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>144</v>
       </c>
@@ -6703,7 +6771,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>145</v>
       </c>
@@ -6726,7 +6794,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>146</v>
       </c>
@@ -6749,7 +6817,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>147</v>
       </c>
@@ -6772,7 +6840,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>148</v>
       </c>
@@ -6795,7 +6863,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>149</v>
       </c>
@@ -6818,7 +6886,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>150</v>
       </c>
@@ -6841,7 +6909,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>151</v>
       </c>
@@ -6864,7 +6932,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>152</v>
       </c>
@@ -6887,7 +6955,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>153</v>
       </c>
@@ -6910,7 +6978,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>154</v>
       </c>
@@ -6933,7 +7001,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>155</v>
       </c>
@@ -6956,7 +7024,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>156</v>
       </c>
@@ -6979,7 +7047,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>157</v>
       </c>
@@ -7002,7 +7070,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>158</v>
       </c>
@@ -7025,7 +7093,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>159</v>
       </c>
@@ -7048,7 +7116,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>160</v>
       </c>
@@ -7071,7 +7139,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>161</v>
       </c>
@@ -7094,7 +7162,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>162</v>
       </c>
@@ -7117,7 +7185,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>163</v>
       </c>
@@ -7140,7 +7208,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>164</v>
       </c>
@@ -7163,7 +7231,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>165</v>
       </c>
@@ -7186,7 +7254,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>166</v>
       </c>
@@ -7209,7 +7277,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>167</v>
       </c>
@@ -7232,7 +7300,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>168</v>
       </c>
@@ -7255,7 +7323,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="375" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" ht="375" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>169</v>
       </c>
@@ -7278,7 +7346,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>170</v>
       </c>
@@ -7301,7 +7369,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>171</v>
       </c>
@@ -7324,7 +7392,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="174" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>172</v>
       </c>
@@ -7347,7 +7415,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>173</v>
       </c>
@@ -7370,7 +7438,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>174</v>
       </c>
@@ -7416,7 +7484,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="178" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>176</v>
       </c>
@@ -7439,7 +7507,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="179" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>177</v>
       </c>
@@ -7462,7 +7530,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="180" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>178</v>
       </c>
@@ -7485,7 +7553,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>179</v>
       </c>
@@ -7508,7 +7576,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>180</v>
       </c>
@@ -7531,7 +7599,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>181</v>
       </c>
@@ -7554,7 +7622,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>182</v>
       </c>
@@ -7577,7 +7645,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="330" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>183</v>
       </c>
@@ -7600,7 +7668,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="345" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:7" ht="345" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>184</v>
       </c>
@@ -7646,7 +7714,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="188" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>186</v>
       </c>
@@ -7669,7 +7737,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="189" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>187</v>
       </c>
@@ -7692,7 +7760,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="190" spans="1:7" ht="255" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:7" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>188</v>
       </c>
@@ -7715,7 +7783,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:7" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>189</v>
       </c>
@@ -7738,7 +7806,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="192" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:7" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>190</v>
       </c>
@@ -7784,7 +7852,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>192</v>
       </c>
@@ -7807,7 +7875,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>193</v>
       </c>
@@ -7830,7 +7898,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="196" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>194</v>
       </c>
@@ -7876,7 +7944,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>196</v>
       </c>
@@ -7899,7 +7967,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="199" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>197</v>
       </c>
@@ -7922,7 +7990,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="200" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>198</v>
       </c>
@@ -7945,7 +8013,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="201" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>199</v>
       </c>
@@ -7968,7 +8036,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="202" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>200</v>
       </c>
@@ -7991,7 +8059,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="203" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>201</v>
       </c>
@@ -8014,7 +8082,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="204" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>202</v>
       </c>
@@ -8037,7 +8105,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="205" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>203</v>
       </c>
@@ -8060,7 +8128,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>204</v>
       </c>
@@ -8083,7 +8151,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="207" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>205</v>
       </c>
@@ -8106,7 +8174,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>206</v>
       </c>
@@ -8129,7 +8197,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>207</v>
       </c>
@@ -8152,7 +8220,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>208</v>
       </c>
@@ -8175,7 +8243,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>209</v>
       </c>
@@ -8198,7 +8266,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:7" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>210</v>
       </c>
@@ -8221,7 +8289,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>211</v>
       </c>
@@ -8244,7 +8312,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>212</v>
       </c>
@@ -8267,7 +8335,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="405" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:7" ht="405" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>213</v>
       </c>
@@ -8290,7 +8358,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>214</v>
       </c>
@@ -8313,7 +8381,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="300" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>215</v>
       </c>
@@ -8336,7 +8404,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="390" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" ht="390" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>216</v>
       </c>
@@ -8359,7 +8427,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="270" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="270" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>217</v>
       </c>
@@ -8382,7 +8450,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" ht="360" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>218</v>
       </c>
@@ -8405,7 +8473,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>219</v>
       </c>
@@ -8428,7 +8496,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>220</v>
       </c>
@@ -8451,7 +8519,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="225" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" ht="225" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>221</v>
       </c>
@@ -8474,7 +8542,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:7" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>222</v>
       </c>
@@ -8520,7 +8588,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>224</v>
       </c>
@@ -8543,7 +8611,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>225</v>
       </c>
@@ -8567,7 +8635,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G227" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="G1:G227" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Иркутская обл."/>
+        <filter val="Иркутская обл., Республика Бурятия"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G217">
     <sortCondition ref="A2:A217"/>
   </sortState>
@@ -8578,10 +8653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21466FB-0E48-4F71-8817-3FE6904DEEA6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8590,24 +8665,28 @@
     <col min="2" max="2" width="49.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="104.42578125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="91.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>801</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>894</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -8615,13 +8694,16 @@
         <v>802</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>885</v>
+        <v>968</v>
       </c>
       <c r="D2" t="s">
-        <v>896</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>895</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -8629,276 +8711,336 @@
         <v>803</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>905</v>
-      </c>
-      <c r="D3" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>903</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>909</v>
-      </c>
-      <c r="D4" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>902</v>
       </c>
-      <c r="D5" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>888</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" t="s">
         <v>889</v>
       </c>
-      <c r="D6" t="s">
-        <v>890</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>892</v>
-      </c>
       <c r="D7" t="s">
-        <v>898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>897</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C8" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D8" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>892</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>899</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" t="s">
         <v>900</v>
       </c>
-      <c r="D9" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>906</v>
-      </c>
-      <c r="D10" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>904</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>911</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>907</v>
-      </c>
-      <c r="D11" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>910</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>914</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>917</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>919</v>
-      </c>
       <c r="D13" s="1" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>916</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>921</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>923</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>926</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>928</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>925</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>955</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>958</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>956</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>958</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E19" s="1" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>962</v>
+        <v>992</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>961</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>964</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>970</v>
+        <v>967</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>982</v>
       </c>
     </row>
   </sheetData>
@@ -8911,8 +9053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ACF4EAF-F69B-487A-A69E-09EA0326EF5A}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8926,10 +9068,10 @@
         <v>801</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -8940,7 +9082,7 @@
         <v>802</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>885</v>
+        <v>968</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -8951,7 +9093,7 @@
         <v>803</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -8959,10 +9101,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -8970,10 +9112,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>902</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -8981,10 +9123,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>888</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -8992,10 +9134,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>891</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -9003,10 +9145,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C8" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9014,10 +9156,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>899</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -9025,10 +9167,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -9036,10 +9178,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -9047,10 +9189,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9058,10 +9200,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>917</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -9069,10 +9211,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -9080,10 +9222,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -9091,10 +9233,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>926</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="105" x14ac:dyDescent="0.25">
@@ -9102,10 +9244,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -9113,10 +9255,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -9124,10 +9266,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -9135,10 +9277,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>962</v>
+        <v>992</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -9146,10 +9288,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -9157,10 +9299,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>
@@ -9173,8 +9315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CA1B08-C4AA-45C3-A90D-FF41C5F0D399}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9189,21 +9331,21 @@
         <v>801</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>886</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>885</v>
+        <v>968</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -9211,10 +9353,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -9222,21 +9364,21 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>902</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -9244,10 +9386,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -9255,10 +9397,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -9266,10 +9408,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>892</v>
+      </c>
+      <c r="C8" t="s">
         <v>893</v>
-      </c>
-      <c r="C8" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -9277,10 +9419,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -9288,10 +9430,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -9299,10 +9441,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9310,10 +9452,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9321,10 +9463,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9332,10 +9474,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -9343,10 +9485,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9354,10 +9496,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9365,10 +9507,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -9376,10 +9518,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9387,10 +9529,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -9398,10 +9540,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>962</v>
+        <v>992</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -9409,10 +9551,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -9420,10 +9562,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
   </sheetData>
@@ -9433,6 +9575,267 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{933BC128-7E89-42E0-8995-6D0075E9A9AF}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="C8" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90AD5810-57C9-40E6-A4CC-C9E8B63D78EA}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -9450,7 +9853,7 @@
         <v>801</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -9458,7 +9861,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9466,7 +9869,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9474,7 +9877,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9482,7 +9885,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -9490,7 +9893,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9498,7 +9901,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -9506,7 +9909,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9514,7 +9917,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9522,7 +9925,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9530,7 +9933,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -9538,7 +9941,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
     </row>
   </sheetData>
@@ -9547,7 +9950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B15F95-1208-4644-B605-305A03285FB0}">
   <dimension ref="A1:B12"/>
   <sheetViews>
@@ -9565,7 +9968,7 @@
         <v>801</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -9573,7 +9976,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -9581,7 +9984,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -9589,7 +9992,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -9597,7 +10000,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -9605,7 +10008,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -9613,7 +10016,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -9621,7 +10024,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -9629,7 +10032,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -9637,7 +10040,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -9645,7 +10048,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -9653,7 +10056,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
   </sheetData>

</xml_diff>